<commit_message>
Workaround for #686 introduced.
</commit_message>
<xml_diff>
--- a/tests/Templates/GroupTagTests_WithHeader.xlsx
+++ b/tests/Templates/GroupTagTests_WithHeader.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ClosedXML\ClosedXML.Report2\tests\Templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="600" yWindow="615" windowWidth="17400" windowHeight="11460"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="Orders">Sheet1!$A$5:$H$6</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -78,11 +83,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <name val="Arial"/>
@@ -304,9 +309,70 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="11">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -426,6 +492,14 @@
       <color rgb="FF9F7CFF"/>
     </mruColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -819,18 +893,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.25"/>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
@@ -838,7 +912,7 @@
     <col min="5" max="10" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="51" customHeight="1">
+    <row r="1" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="18" t="s">
         <v>7</v>
@@ -850,7 +924,7 @@
       <c r="G1" s="19"/>
       <c r="H1" s="19"/>
     </row>
-    <row r="2" spans="1:10" ht="12.75">
+    <row r="2" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -860,7 +934,7 @@
       <c r="G2" s="4"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="12">
+    <row r="3" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="1"/>
@@ -872,7 +946,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="22.5">
+    <row r="4" spans="1:10" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="6" t="s">
         <v>6</v>
@@ -896,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="11.25" customHeight="1">
+    <row r="5" spans="1:10" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="11" t="s">
         <v>16</v>
@@ -923,7 +997,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="17" t="s">
         <v>14</v>
@@ -947,7 +1021,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -961,12 +1035,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -998,22 +1072,17 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <conditionalFormatting sqref="C6:H6">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$G6&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="4" stopIfTrue="1">
       <formula>$G6&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
-      <formula>$G6&lt;&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="1" stopIfTrue="1">
       <formula>$G6&lt;&gt;0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>